<commit_message>
tmp updated for islet motif figure
</commit_message>
<xml_diff>
--- a/test/pd.sub.rank.anno.check.xlsx
+++ b/test/pd.sub.rank.anno.check.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/frank/github/atacMotif/test/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A4BA3C08-D09E-5748-83A9-144EF6460E60}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="38" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DA69BB77-95B0-D644-A67F-70C6596651C5}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="38" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-28600" yWindow="3860" windowWidth="27640" windowHeight="16940" activeTab="1" xr2:uid="{37029347-5E09-A94D-9496-FD89E728F0DC}"/>
   </bookViews>
@@ -1006,6 +1006,9 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{368E41BC-021E-0548-AA6D-37D8530B5F99}">
+  <sheetPr>
+    <pageSetUpPr fitToPage="1"/>
+  </sheetPr>
   <dimension ref="A1:S18"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -2082,15 +2085,19 @@
     <hyperlink ref="B1" r:id="rId1" display="http://sf.id/" xr:uid="{CED54415-A138-3742-ACA9-BA5D494D9BDE}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup scale="48" orientation="landscape" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F575AF9C-7187-8F40-8864-2C4122470247}">
+  <sheetPr>
+    <pageSetUpPr fitToPage="1"/>
+  </sheetPr>
   <dimension ref="A1:S18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F33" sqref="F33"/>
+      <selection activeCell="P17" sqref="P17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -3163,5 +3170,6 @@
     <hyperlink ref="B1" r:id="rId1" display="http://sf.id/" xr:uid="{C3AFD762-3B81-4D4A-AD4C-C59330C07894}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup scale="48" orientation="landscape" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>
 </file>
</xml_diff>